<commit_message>
Just to make everything is pushed to git
</commit_message>
<xml_diff>
--- a/results_env_training.xlsx
+++ b/results_env_training.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masterproef_code\LSSVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD372113-FCA4-43F9-B866-EFDA39A8252F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4879BB59-5346-4309-8510-ED3FBFB134CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6DD0E1EA-E87A-423C-9521-544A3F429BB3}"/>
   </bookViews>
@@ -28224,9 +28224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65449D9-57ED-487D-A21A-C25D0AC394A7}">
   <dimension ref="A1:AP258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AO252" sqref="AO252"/>
+      <selection pane="topRight" activeCell="AO196" sqref="AO196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32572,7 +32572,7 @@
         <v>1</v>
       </c>
       <c r="AC69" s="20" t="str">
-        <f t="shared" ref="AC69:AM69" si="38">_xlfn.CONCAT(TEXT(AC39,"0,00%")," ± ",TEXT(AC9,"0,00%"))</f>
+        <f t="shared" ref="AC69" si="38">_xlfn.CONCAT(TEXT(AC39,"0,00%")," ± ",TEXT(AC9,"0,00%"))</f>
         <v>78,68% ± 0,38%</v>
       </c>
       <c r="AD69" s="20" t="str">
@@ -33034,7 +33034,7 @@
         <v>2</v>
       </c>
       <c r="AC75" s="20" t="str">
-        <f t="shared" ref="AC75:AM75" si="45">_xlfn.CONCAT(TEXT(AC45,"0,00%")," ± ",TEXT(AC15,"0,00%"))</f>
+        <f t="shared" ref="AC75" si="45">_xlfn.CONCAT(TEXT(AC45,"0,00%")," ± ",TEXT(AC15,"0,00%"))</f>
         <v>82,75% ± 0,43%</v>
       </c>
       <c r="AD75" s="20" t="str">
@@ -33593,7 +33593,7 @@
         <v>7</v>
       </c>
       <c r="AC83" s="20" t="str">
-        <f t="shared" ref="AC83:AM83" si="52">_xlfn.CONCAT(TEXT(AC53,"0,00%")," ± ",TEXT(AC23,"0,00%"))</f>
+        <f t="shared" ref="AC83" si="52">_xlfn.CONCAT(TEXT(AC53,"0,00%")," ± ",TEXT(AC23,"0,00%"))</f>
         <v>91,97% ± 0,30%</v>
       </c>
       <c r="AD83" s="20" t="str">
@@ -42145,10 +42145,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8560AD5C-2B64-4578-8B47-159958EC7742}">
   <dimension ref="A1:AM258"/>
   <sheetViews>
-    <sheetView topLeftCell="A218" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
       <selection activeCell="A160" sqref="A160"/>
-      <selection pane="topRight" activeCell="AD88" sqref="AD88"/>
+      <selection pane="topRight" activeCell="AD220" sqref="AD220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>